<commit_message>
global refactor unique lists update
</commit_message>
<xml_diff>
--- a/Megafon .xlsx
+++ b/Megafon .xlsx
@@ -12,29 +12,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>9375204365</t>
   </si>
   <si>
-    <t>9375204823</t>
-  </si>
-  <si>
-    <t>9375205264</t>
-  </si>
-  <si>
-    <t>9375797946</t>
-  </si>
-  <si>
-    <t>9375204391</t>
-  </si>
-  <si>
     <t>9375204382</t>
   </si>
   <si>
     <t>9375204397</t>
   </si>
   <si>
+    <t>9375204518</t>
+  </si>
+  <si>
     <t>9375204529</t>
   </si>
   <si>
@@ -47,48 +38,15 @@
     <t>9375204537</t>
   </si>
   <si>
-    <t>9375204542</t>
-  </si>
-  <si>
-    <t>9375204551</t>
-  </si>
-  <si>
     <t>9375204553</t>
   </si>
   <si>
-    <t>9375205280</t>
-  </si>
-  <si>
-    <t>9375205270</t>
-  </si>
-  <si>
     <t>9375205286</t>
   </si>
   <si>
     <t>9375205296</t>
   </si>
   <si>
-    <t>9375204569</t>
-  </si>
-  <si>
-    <t>9375204580</t>
-  </si>
-  <si>
-    <t>9375204572</t>
-  </si>
-  <si>
-    <t>9375204578</t>
-  </si>
-  <si>
-    <t>9375204573</t>
-  </si>
-  <si>
-    <t>9375204577</t>
-  </si>
-  <si>
-    <t>9375204576</t>
-  </si>
-  <si>
     <t>9375204585</t>
   </si>
   <si>
@@ -98,12 +56,6 @@
     <t>9375204605</t>
   </si>
   <si>
-    <t>9375204601</t>
-  </si>
-  <si>
-    <t>9375205308</t>
-  </si>
-  <si>
     <t>9375204608</t>
   </si>
   <si>
@@ -131,7 +83,7 @@
     <t>9375823270</t>
   </si>
   <si>
-    <t>9372921232</t>
+    <t>9372921150</t>
   </si>
   <si>
     <t>9372920857</t>
@@ -146,6 +98,78 @@
     <t>9372975879</t>
   </si>
   <si>
+    <t>9372921364</t>
+  </si>
+  <si>
+    <t>9375203244</t>
+  </si>
+  <si>
+    <t>9375814225</t>
+  </si>
+  <si>
+    <t>9397498073</t>
+  </si>
+  <si>
+    <t>9372919584</t>
+  </si>
+  <si>
+    <t>9376268702</t>
+  </si>
+  <si>
+    <t>9376258078</t>
+  </si>
+  <si>
+    <t>9375204625</t>
+  </si>
+  <si>
+    <t>9375204613</t>
+  </si>
+  <si>
+    <t>9375204623</t>
+  </si>
+  <si>
+    <t>9375204622</t>
+  </si>
+  <si>
+    <t>9375204619</t>
+  </si>
+  <si>
+    <t>9372914234</t>
+  </si>
+  <si>
+    <t>9375204654</t>
+  </si>
+  <si>
+    <t>9375204651</t>
+  </si>
+  <si>
+    <t>9375204649</t>
+  </si>
+  <si>
+    <t>9375204513</t>
+  </si>
+  <si>
+    <t>9372919472</t>
+  </si>
+  <si>
+    <t>9375204634</t>
+  </si>
+  <si>
+    <t>9375204632</t>
+  </si>
+  <si>
+    <t>9375204653</t>
+  </si>
+  <si>
+    <t>9372912146</t>
+  </si>
+  <si>
+    <t>9372912164</t>
+  </si>
+  <si>
+    <t>9372912104</t>
+  </si>
+  <si>
     <t>9274559669</t>
   </si>
   <si>
@@ -158,18 +182,9 @@
     <t>9297614242</t>
   </si>
   <si>
-    <t>9372838666</t>
-  </si>
-  <si>
     <t>9272403636</t>
   </si>
   <si>
-    <t>9372951414</t>
-  </si>
-  <si>
-    <t>9297642828</t>
-  </si>
-  <si>
     <t>9274593737</t>
   </si>
   <si>
@@ -278,6 +293,18 @@
     <t>9376293131</t>
   </si>
   <si>
+    <t>9376294747</t>
+  </si>
+  <si>
+    <t>9397409696</t>
+  </si>
+  <si>
+    <t>9274716969</t>
+  </si>
+  <si>
+    <t>9377715522</t>
+  </si>
+  <si>
     <t>9397454884</t>
   </si>
   <si>
@@ -287,9 +314,6 @@
     <t>9375852244</t>
   </si>
   <si>
-    <t>9377715522</t>
-  </si>
-  <si>
     <t>9274758855</t>
   </si>
   <si>
@@ -330,6 +354,9 @@
   </si>
   <si>
     <t>9274888843</t>
+  </si>
+  <si>
+    <t>9370011115</t>
   </si>
   <si>
     <t>9375937799</t>
@@ -494,7 +521,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B146"/>
+  <dimension ref="A1:B155"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -857,7 +884,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="46">
@@ -865,7 +892,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="47">
@@ -873,7 +900,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="48">
@@ -881,7 +908,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="49">
@@ -889,7 +916,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="50">
@@ -897,7 +924,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="51">
@@ -905,7 +932,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="52">
@@ -913,7 +940,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>800.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="53">
@@ -1209,7 +1236,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>4000.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="90">
@@ -1217,7 +1244,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>4000.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="91">
@@ -1225,7 +1252,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>4000.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="92">
@@ -1233,7 +1260,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>4000.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="93">
@@ -1241,7 +1268,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>4000.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="94">
@@ -1249,7 +1276,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>4000.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="95">
@@ -1257,7 +1284,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>4000.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="96">
@@ -1265,7 +1292,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>4000.0</v>
+        <v>800.0</v>
       </c>
     </row>
     <row r="97">
@@ -1561,7 +1588,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="134">
@@ -1569,7 +1596,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="135">
@@ -1577,7 +1604,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="136">
@@ -1585,7 +1612,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="137">
@@ -1593,7 +1620,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="138">
@@ -1601,7 +1628,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="139">
@@ -1609,7 +1636,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="140">
@@ -1617,7 +1644,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="141">
@@ -1625,7 +1652,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="n">
-        <v>5000.0</v>
+        <v>4000.0</v>
       </c>
     </row>
     <row r="142">
@@ -1657,7 +1684,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="n">
-        <v>15000.0</v>
+        <v>5000.0</v>
       </c>
     </row>
     <row r="146">
@@ -1665,6 +1692,78 @@
         <v>145</v>
       </c>
       <c r="B146" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>146</v>
+      </c>
+      <c r="B147" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>147</v>
+      </c>
+      <c r="B148" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>148</v>
+      </c>
+      <c r="B149" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>149</v>
+      </c>
+      <c r="B150" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>150</v>
+      </c>
+      <c r="B151" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>151</v>
+      </c>
+      <c r="B152" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>152</v>
+      </c>
+      <c r="B153" t="n">
+        <v>5000.0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>153</v>
+      </c>
+      <c r="B154" t="n">
+        <v>15000.0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>154</v>
+      </c>
+      <c r="B155" t="n">
         <v>15000.0</v>
       </c>
     </row>

</xml_diff>